<commit_message>
Reglé le bug fonctionnalité 8 et 9. (Affichage erreur)
</commit_message>
<xml_diff>
--- a/TestFiles/Tests.xlsx
+++ b/TestFiles/Tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>Description</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>1) Me dit que le jour weekend 1 est une journée de vacances Note: le 480 minutes a été pris en comte ici</t>
   </si>
   <si>
     <t>Tester que le congé férié et bien pris comme temps "bureau"</t>
@@ -533,7 +530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -562,6 +559,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -688,7 +687,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -702,6 +701,8 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1047,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1133,7 +1134,7 @@
         <v>43</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18">
@@ -1170,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="32" t="str">
-        <f t="shared" ref="D6:D28" si="0">HYPERLINK(CONCATENATE("F_",B6,".json"),CONCATENATE("F_",B6,".json"))</f>
+        <f t="shared" ref="D6:D26" si="0">HYPERLINK(CONCATENATE("F_",B6,".json"),CONCATENATE("F_",B6,".json"))</f>
         <v>F_4.json</v>
       </c>
       <c r="E6" s="33" t="s">
@@ -1256,18 +1257,18 @@
       <c r="A10" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="30">
         <v>8</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="15" t="str">
+      <c r="D10" s="32" t="str">
         <f t="shared" si="0"/>
         <v>F_8.json</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>55</v>
+      <c r="E10" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>36</v>
@@ -1278,18 +1279,18 @@
     </row>
     <row r="11" spans="1:9" ht="96">
       <c r="A11" s="39"/>
-      <c r="B11" s="13">
+      <c r="B11" s="30">
         <v>9</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="15" t="str">
+      <c r="D11" s="32" t="str">
         <f t="shared" si="0"/>
         <v>F_9.json</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>55</v>
+      <c r="E11" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>41</v>
@@ -1376,7 +1377,7 @@
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>50</v>
@@ -1430,7 +1431,7 @@
         <v>F_16.json</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18">
@@ -1462,7 +1463,7 @@
         <v>F_18.json</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18">
@@ -1475,7 +1476,7 @@
       </c>
       <c r="D21" s="28"/>
       <c r="E21" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32">
@@ -1552,16 +1553,16 @@
     </row>
     <row r="27" spans="1:5" ht="18">
       <c r="A27" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" s="30">
         <v>25</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" s="33" t="s">
         <v>53</v>
@@ -1573,10 +1574,10 @@
         <v>26</v>
       </c>
       <c r="C28" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="36" t="s">
         <v>57</v>
-      </c>
-      <c r="D28" s="36" t="s">
-        <v>58</v>
       </c>
       <c r="E28" s="33" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
Regler bogue F_16: Plusieurs messages d'erreurs pour le congé parental (un seul congé par semaine)
</commit_message>
<xml_diff>
--- a/TestFiles/Tests.xlsx
+++ b/TestFiles/Tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Description</t>
   </si>
@@ -199,9 +199,6 @@
   </si>
   <si>
     <t>Autres tests</t>
-  </si>
-  <si>
-    <t>Plusieurs messages d'erreurs pour le congé parental (un seul congé par semaine)</t>
   </si>
   <si>
     <t>&lt; 2000</t>
@@ -530,7 +527,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -559,6 +556,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -687,7 +689,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -703,6 +705,11 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1048,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1134,7 +1141,7 @@
         <v>43</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18">
@@ -1420,18 +1427,18 @@
     </row>
     <row r="18" spans="1:5" ht="80">
       <c r="A18" s="40"/>
-      <c r="B18" s="13">
+      <c r="B18" s="30">
         <v>16</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="15" t="str">
+      <c r="D18" s="32" t="str">
         <f t="shared" si="0"/>
         <v>F_16.json</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>60</v>
+      <c r="E18" s="35" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18">
@@ -1463,7 +1470,7 @@
         <v>F_18.json</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18">
@@ -1476,7 +1483,7 @@
       </c>
       <c r="D21" s="28"/>
       <c r="E21" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32">

</xml_diff>

<commit_message>
Règler bogue F_18 : on suppose que le 41.5 heures est du temps au bureau
</commit_message>
<xml_diff>
--- a/TestFiles/Tests.xlsx
+++ b/TestFiles/Tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>Description</t>
   </si>
@@ -204,17 +204,17 @@
     <t>&lt; 2000</t>
   </si>
   <si>
-    <t>json 2525 minutes temps doit être &lt; 2490</t>
-  </si>
-  <si>
     <t>Annuler</t>
+  </si>
+  <si>
+    <t>Tester la non-conformité du fichier JSON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -289,6 +289,13 @@
       <name val="Cambria"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -296,12 +303,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -345,8 +346,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -514,16 +521,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -564,7 +578,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -573,9 +587,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -594,18 +605,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,69 +623,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="27" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -1053,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1075,163 +1096,163 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" thickBot="1"/>
     <row r="2" spans="1:9" ht="26" customHeight="1" thickTop="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="40" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="38"/>
-      <c r="B4" s="23">
+      <c r="A4" s="33"/>
+      <c r="B4" s="18">
         <v>2</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18">
-      <c r="A5" s="38"/>
-      <c r="B5" s="30">
+      <c r="A5" s="33"/>
+      <c r="B5" s="25">
         <v>3</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="32" t="str">
+      <c r="D5" s="27" t="str">
         <f>HYPERLINK(CONCATENATE("F_",B5,".json"),CONCATENATE("F_",B5,".json"))</f>
         <v>F_3.json</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F5" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18">
-      <c r="A6" s="38"/>
-      <c r="B6" s="30">
+      <c r="A6" s="33"/>
+      <c r="B6" s="25">
         <v>4</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="32" t="str">
+      <c r="D6" s="27" t="str">
         <f t="shared" ref="D6:D26" si="0">HYPERLINK(CONCATENATE("F_",B6,".json"),CONCATENATE("F_",B6,".json"))</f>
         <v>F_4.json</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="19" thickBot="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="30">
+      <c r="A7" s="33"/>
+      <c r="B7" s="25">
         <v>5</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="32" t="str">
+      <c r="D7" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_5.json</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>6000</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="34" thickTop="1" thickBot="1">
-      <c r="A8" s="38"/>
-      <c r="B8" s="30">
+      <c r="A8" s="33"/>
+      <c r="B8" s="25">
         <v>6</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="32" t="str">
+      <c r="D8" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_6.json</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="30" t="s">
         <v>53</v>
       </c>
       <c r="F8" t="s">
@@ -1239,364 +1260,378 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="33" thickTop="1">
-      <c r="A9" s="38"/>
-      <c r="B9" s="30">
+      <c r="A9" s="33"/>
+      <c r="B9" s="25">
         <v>7</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="32" t="str">
+      <c r="D9" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_7.json</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="30" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="96">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="25">
         <v>8</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="32" t="str">
+      <c r="D10" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_8.json</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="96">
-      <c r="A11" s="39"/>
-      <c r="B11" s="30">
+      <c r="A11" s="34"/>
+      <c r="B11" s="25">
         <v>9</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="32" t="str">
+      <c r="D11" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_9.json</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <v>999</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="96">
-      <c r="A12" s="39"/>
-      <c r="B12" s="30">
+      <c r="A12" s="34"/>
+      <c r="B12" s="25">
         <v>10</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="32" t="str">
+      <c r="D12" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_10.json</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <v>998</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="32">
-      <c r="A13" s="39"/>
-      <c r="B13" s="30">
+      <c r="A13" s="34"/>
+      <c r="B13" s="25">
         <v>11</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="32" t="str">
+      <c r="D13" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_11.json</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="9">
         <v>997</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="64">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="25">
         <v>12</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="32" t="str">
+      <c r="D14" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_12.json</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="9">
         <v>996</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="81" thickBot="1">
-      <c r="A15" s="40"/>
-      <c r="B15" s="23">
+      <c r="A15" s="35"/>
+      <c r="B15" s="18">
         <v>13</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
         <v>777</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="65" thickTop="1">
-      <c r="A16" s="40"/>
-      <c r="B16" s="30">
+      <c r="A16" s="35"/>
+      <c r="B16" s="25">
         <v>14</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="32" t="str">
+      <c r="D16" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_14.json</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="80">
-      <c r="A17" s="40"/>
-      <c r="B17" s="30">
+      <c r="A17" s="35"/>
+      <c r="B17" s="25">
         <v>15</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="32" t="str">
+      <c r="D17" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_15.json</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="80">
-      <c r="A18" s="40"/>
-      <c r="B18" s="30">
+      <c r="A18" s="35"/>
+      <c r="B18" s="25">
         <v>16</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="32" t="str">
+      <c r="D18" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_16.json</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18">
-      <c r="A19" s="40"/>
-      <c r="B19" s="30">
+      <c r="A19" s="35"/>
+      <c r="B19" s="25">
         <v>17</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="32" t="str">
+      <c r="D19" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_17.json</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32">
-      <c r="A20" s="40"/>
-      <c r="B20" s="13">
+      <c r="A20" s="35"/>
+      <c r="B20" s="25">
         <v>18</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="15" t="str">
+      <c r="D20" s="27" t="str">
         <f t="shared" si="0"/>
         <v>F_18.json</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18">
+      <c r="A21" s="35"/>
+      <c r="B21" s="18">
+        <v>19</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18">
-      <c r="A21" s="40"/>
-      <c r="B21" s="23">
-        <v>19</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
     <row r="22" spans="1:5" ht="32">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>20</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="17" t="str">
+      <c r="D22" s="12" t="str">
         <f t="shared" si="0"/>
         <v>F_20.json</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" ht="18">
-      <c r="A23" s="41"/>
-      <c r="B23" s="6">
+      <c r="A23" s="36"/>
+      <c r="B23" s="5">
         <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="17" t="str">
+      <c r="D23" s="12" t="str">
         <f t="shared" si="0"/>
         <v>F_21.json</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" ht="32">
-      <c r="A24" s="41"/>
-      <c r="B24" s="6">
+      <c r="A24" s="36"/>
+      <c r="B24" s="5">
         <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="17" t="str">
+      <c r="D24" s="12" t="str">
         <f t="shared" si="0"/>
         <v>F_22.json</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" ht="18">
-      <c r="A25" s="41"/>
-      <c r="B25" s="6">
+      <c r="A25" s="36"/>
+      <c r="B25" s="5">
         <v>23</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="17" t="str">
+      <c r="D25" s="12" t="str">
         <f t="shared" si="0"/>
         <v>F_23.json</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" ht="48">
-      <c r="A26" s="42"/>
-      <c r="B26" s="19">
+      <c r="A26" s="37"/>
+      <c r="B26" s="14">
         <v>24</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="21" t="str">
+      <c r="D26" s="16" t="str">
         <f t="shared" si="0"/>
         <v>F_24.json</v>
       </c>
-      <c r="E26" s="22"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" ht="18">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="25">
         <v>25</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="28" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18">
-      <c r="A28" s="44"/>
-      <c r="B28" s="30">
+      <c r="A28" s="42"/>
+      <c r="B28" s="25">
         <v>26</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="28" t="s">
         <v>53</v>
       </c>
+    </row>
+    <row r="29" spans="1:5" ht="18">
+      <c r="A29" s="43"/>
+      <c r="B29" s="44">
+        <v>27</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="47" t="str">
+        <f t="shared" ref="D29" si="1">HYPERLINK(CONCATENATE("F_",B29,".json"),CONCATENATE("F_",B29,".json"))</f>
+        <v>F_27.json</v>
+      </c>
+      <c r="E29" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A27:A29"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A21"/>
     <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A27:A28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Règler bogue F_27 : Est feuille valide même si le fichier JSON ne l'est pas, ne crée pas de fichier jSON vide
</commit_message>
<xml_diff>
--- a/TestFiles/Tests.xlsx
+++ b/TestFiles/Tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Description</t>
   </si>
@@ -297,7 +297,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,12 +346,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -578,7 +572,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -697,16 +691,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1076,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1613,17 +1598,19 @@
     </row>
     <row r="29" spans="1:5" ht="18">
       <c r="A29" s="43"/>
-      <c r="B29" s="44">
+      <c r="B29" s="25">
         <v>27</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="47" t="str">
+      <c r="D29" s="44" t="str">
         <f t="shared" ref="D29" si="1">HYPERLINK(CONCATENATE("F_",B29,".json"),CONCATENATE("F_",B29,".json"))</f>
         <v>F_27.json</v>
       </c>
-      <c r="E29" s="46"/>
+      <c r="E29" s="30" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Ajout test JsonFabriqueObjTest pour les différents types d'employé
</commit_message>
<xml_diff>
--- a/TestFiles/Tests.xlsx
+++ b/TestFiles/Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33560" yWindow="-440" windowWidth="25640" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="34140" yWindow="1460" windowWidth="25640" windowHeight="20480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tests INF2015" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>Congé férié</t>
   </si>
   <si>
-    <t>Production</t>
-  </si>
-  <si>
     <t>Exploitation</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>Tester la non-conformité du fichier JSON</t>
+  </si>
+  <si>
+    <t>Développement</t>
   </si>
 </sst>
 </file>
@@ -660,6 +660,25 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,25 +693,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -1061,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1073,7 +1073,7 @@
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="3.5" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
@@ -1081,19 +1081,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" thickBot="1"/>
     <row r="2" spans="1:9" ht="26" customHeight="1" thickTop="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="35" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1105,7 +1105,7 @@
       <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="18">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="40" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="18">
@@ -1116,10 +1116,10 @@
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>34</v>
@@ -1129,7 +1129,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="33"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="18">
         <v>2</v>
       </c>
@@ -1138,20 +1138,20 @@
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18">
-      <c r="A5" s="33"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="25">
         <v>3</v>
       </c>
@@ -1163,20 +1163,20 @@
         <v>F_3.json</v>
       </c>
       <c r="E5" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
       <c r="G5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="18">
-      <c r="A6" s="33"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="25">
         <v>4</v>
       </c>
@@ -1188,20 +1188,20 @@
         <v>F_4.json</v>
       </c>
       <c r="E6" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
         <v>53</v>
       </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="7" spans="1:9" ht="19" thickBot="1">
-      <c r="A7" s="33"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="25">
         <v>5</v>
       </c>
@@ -1213,20 +1213,20 @@
         <v>F_5.json</v>
       </c>
       <c r="E7" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
         <v>53</v>
       </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
       <c r="G7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" s="11">
         <v>6000</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="34" thickTop="1" thickBot="1">
-      <c r="A8" s="33"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="25">
         <v>6</v>
       </c>
@@ -1238,14 +1238,14 @@
         <v>F_6.json</v>
       </c>
       <c r="E8" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="9" spans="1:9" ht="33" thickTop="1">
-      <c r="A9" s="33"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="25">
         <v>7</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>F_7.json</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>35</v>
@@ -1267,7 +1267,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="96">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="25">
@@ -1281,7 +1281,7 @@
         <v>F_8.json</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>36</v>
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="96">
-      <c r="A11" s="34"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="25">
         <v>9</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>F_9.json</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>41</v>
@@ -1313,7 +1313,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="96">
-      <c r="A12" s="34"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="25">
         <v>10</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>F_10.json</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>42</v>
@@ -1335,7 +1335,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="32">
-      <c r="A13" s="34"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="25">
         <v>11</v>
       </c>
@@ -1347,17 +1347,17 @@
         <v>F_11.json</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="9">
         <v>997</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="64">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="25">
@@ -1371,17 +1371,17 @@
         <v>F_12.json</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H14" s="9">
         <v>996</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="81" thickBot="1">
-      <c r="A15" s="35"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="18">
         <v>13</v>
       </c>
@@ -1390,17 +1390,17 @@
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H15" s="11">
         <v>777</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="65" thickTop="1">
-      <c r="A16" s="35"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="25">
         <v>14</v>
       </c>
@@ -1412,11 +1412,11 @@
         <v>F_14.json</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="80">
-      <c r="A17" s="35"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="25">
         <v>15</v>
       </c>
@@ -1428,11 +1428,11 @@
         <v>F_15.json</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="80">
-      <c r="A18" s="35"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="25">
         <v>16</v>
       </c>
@@ -1444,11 +1444,11 @@
         <v>F_16.json</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18">
-      <c r="A19" s="35"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="25">
         <v>17</v>
       </c>
@@ -1460,11 +1460,11 @@
         <v>F_17.json</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32">
-      <c r="A20" s="35"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="25">
         <v>18</v>
       </c>
@@ -1476,11 +1476,11 @@
         <v>F_18.json</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18">
-      <c r="A21" s="35"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="18">
         <v>19</v>
       </c>
@@ -1489,11 +1489,11 @@
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="32">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="43" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="5">
@@ -1509,7 +1509,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" ht="18">
-      <c r="A23" s="36"/>
+      <c r="A23" s="43"/>
       <c r="B23" s="5">
         <v>21</v>
       </c>
@@ -1523,7 +1523,7 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" ht="32">
-      <c r="A24" s="36"/>
+      <c r="A24" s="43"/>
       <c r="B24" s="5">
         <v>22</v>
       </c>
@@ -1537,7 +1537,7 @@
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" ht="18">
-      <c r="A25" s="36"/>
+      <c r="A25" s="43"/>
       <c r="B25" s="5">
         <v>23</v>
       </c>
@@ -1551,7 +1551,7 @@
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" ht="48">
-      <c r="A26" s="37"/>
+      <c r="A26" s="44"/>
       <c r="B26" s="14">
         <v>24</v>
       </c>
@@ -1565,51 +1565,51 @@
       <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" ht="18">
-      <c r="A27" s="41" t="s">
-        <v>59</v>
+      <c r="A27" s="37" t="s">
+        <v>58</v>
       </c>
       <c r="B27" s="25">
         <v>25</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18">
-      <c r="A28" s="42"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="25">
         <v>26</v>
       </c>
       <c r="C28" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="31" t="s">
-        <v>57</v>
-      </c>
       <c r="E28" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18">
-      <c r="A29" s="43"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="25">
         <v>27</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="44" t="str">
+        <v>61</v>
+      </c>
+      <c r="D29" s="36" t="str">
         <f t="shared" ref="D29" si="1">HYPERLINK(CONCATENATE("F_",B29,".json"),CONCATENATE("F_",B29,".json"))</f>
         <v>F_27.json</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>